<commit_message>
Added raw data to correlation_covariance
</commit_message>
<xml_diff>
--- a/data/esempi_correlazione_covarianza.xlsx
+++ b/data/esempi_correlazione_covarianza.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alex/Code/IULM/IULM_DDM2324_Notebooks/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C9AE77EE-6FA3-514D-BAD7-738E3A14D229}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFD9307B-4A0D-7848-9B5A-602B118AB02C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1180" yWindow="1500" windowWidth="27240" windowHeight="15940" xr2:uid="{7B3A289D-CC59-9B43-B9BA-8D7C1EFC1767}"/>
+    <workbookView xWindow="1180" yWindow="1500" windowWidth="27240" windowHeight="15940" activeTab="1" xr2:uid="{7B3A289D-CC59-9B43-B9BA-8D7C1EFC1767}"/>
   </bookViews>
   <sheets>
     <sheet name="Correlazione Positiva" sheetId="1" r:id="rId1"/>
-    <sheet name="Correlazione Negativa" sheetId="2" r:id="rId2"/>
+    <sheet name="Data_1" sheetId="3" r:id="rId2"/>
+    <sheet name="Correlazione Negativa" sheetId="2" r:id="rId3"/>
+    <sheet name="Data_2" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
   <si>
     <t>Età</t>
   </si>
@@ -64,6 +66,9 @@
   <si>
     <t>Standard Deviation</t>
   </si>
+  <si>
+    <t>P-value</t>
+  </si>
 </sst>
 </file>
 
@@ -72,7 +77,7 @@
   <numFmts count="1">
     <numFmt numFmtId="169" formatCode="0.0"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -85,6 +90,22 @@
       <i/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -119,7 +140,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -131,6 +152,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3252,10 +3279,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B3655C6-37E8-F043-A31F-181D60BEA486}">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="B1:C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3410,6 +3437,11 @@
         <v>0.72304526925451473</v>
       </c>
     </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -3418,11 +3450,138 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13E7DB78-9F92-684A-A46C-670149B0404D}">
+  <dimension ref="A1:B14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="6">
+        <v>9</v>
+      </c>
+      <c r="B2" s="6">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="6">
+        <v>12</v>
+      </c>
+      <c r="B3" s="6">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="6">
+        <v>15</v>
+      </c>
+      <c r="B4" s="6">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="6">
+        <v>15</v>
+      </c>
+      <c r="B5" s="6">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="6">
+        <v>4</v>
+      </c>
+      <c r="B6" s="6">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="6">
+        <v>7</v>
+      </c>
+      <c r="B7" s="6">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="6">
+        <v>18</v>
+      </c>
+      <c r="B8" s="6">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="6">
+        <v>19</v>
+      </c>
+      <c r="B9" s="6">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="6">
+        <v>20</v>
+      </c>
+      <c r="B10" s="6">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="6">
+        <v>32</v>
+      </c>
+      <c r="B11" s="6">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="6">
+        <v>45</v>
+      </c>
+      <c r="B12" s="6">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="6">
+        <v>35</v>
+      </c>
+      <c r="B13" s="6">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="6">
+        <v>67</v>
+      </c>
+      <c r="B14" s="6">
+        <v>181</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0D238BC-B7DB-1042-B7F2-F37EAA67366B}">
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="C10" sqref="B1:C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3558,4 +3717,99 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA77A0DB-46C6-344D-98DE-77F2CA944F8B}">
+  <dimension ref="A1:B10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>30000</v>
+      </c>
+      <c r="B2">
+        <v>34484</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>40000</v>
+      </c>
+      <c r="B3">
+        <v>38583</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>42000</v>
+      </c>
+      <c r="B4">
+        <v>36158</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>70000</v>
+      </c>
+      <c r="B5">
+        <v>33855</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>115000</v>
+      </c>
+      <c r="B6">
+        <v>27025</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>230000</v>
+      </c>
+      <c r="B7">
+        <v>14950</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>324000</v>
+      </c>
+      <c r="B8">
+        <v>7384</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>110000</v>
+      </c>
+      <c r="B9">
+        <v>26452</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>99000</v>
+      </c>
+      <c r="B10">
+        <v>28976</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>